<commit_message>
caricato l'esercizio in file .xlsx, .pdf, .png
</commit_message>
<xml_diff>
--- a/db-first.xlsx
+++ b/db-first.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Boolean\Esercitazioni\08 - Agosto\db-first\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871D3147-B020-4CF9-97CD-E78D4C8E2D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,126 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+  <si>
+    <t>Modellizzare la struttura di una tabella per memorizzare tutti i dati riguardanti delle auto usate messe in vendita da un concessionario</t>
+  </si>
+  <si>
+    <t>Car_id</t>
+  </si>
+  <si>
+    <t>Casa_automobilistica</t>
+  </si>
+  <si>
+    <t>Modello</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>Danni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anno </t>
+  </si>
+  <si>
+    <t>Potenza</t>
+  </si>
+  <si>
+    <t>Chilometraggio</t>
+  </si>
+  <si>
+    <t>Carburante</t>
+  </si>
+  <si>
+    <t>BIGINT</t>
+  </si>
+  <si>
+    <t>Varchar (30)</t>
+  </si>
+  <si>
+    <t>Varchar (50)</t>
+  </si>
+  <si>
+    <t>Float(7,2)</t>
+  </si>
+  <si>
+    <t>Float(6,3)</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>Per il carburante ho utilizzato TINYINT per salvare un valore Booleano. In questo caso se è Diesel o Benzina.</t>
+  </si>
+  <si>
+    <t>Anche per i danni ho utilizzato TINYINT per salvare un valore Booleano. In questo caso se presenta o meno danni.</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>Targa</t>
+  </si>
+  <si>
+    <t>Varchar(7)</t>
+  </si>
+  <si>
+    <t>NOT NULL -- UNIQUE</t>
+  </si>
+  <si>
+    <t>Informazioni</t>
+  </si>
+  <si>
+    <t>Descrizione_interni</t>
+  </si>
+  <si>
+    <t>Varchar(50)</t>
+  </si>
+  <si>
+    <t>Paese_origine</t>
+  </si>
+  <si>
+    <t>Varchar(20)</t>
+  </si>
+  <si>
+    <t>Numero_sedili</t>
+  </si>
+  <si>
+    <t>Tappezzeria_originale</t>
+  </si>
+  <si>
+    <t>Per la tappezzeria_originale ho utilizzato TINYINT per salvare un valore Booleano. In questo caso se ha o meno la tappezzeria originale</t>
+  </si>
+  <si>
+    <t>Primary_Key -- AUTO_INCREMENT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,11 +166,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +456,318 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C6:F6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>